<commit_message>
Added more EchoProto template tests
</commit_message>
<xml_diff>
--- a/Resources/data/Reagents.xlsx
+++ b/Resources/data/Reagents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/b6068776_newcastle_ac_uk/Documents/Nextcloud/Private/Automation/Automation_Protocols/BiomationScripter/Resources/For Docs/Labware_Layout_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/b6068776_newcastle_ac_uk/Documents/Nextcloud/Private/Automation/Automation_Protocols/BiomationScripter/Resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{9DCC8006-8A84-4BAF-9E51-97357D0F31D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABCC0C30-0915-424F-BAF5-C017C77CD8B6}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{9DCC8006-8A84-4BAF-9E51-97357D0F31D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9ECF165-D422-4B1F-A648-770CB8588977}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4176" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9F5E6FB9-32EF-42A5-B114-36A33DEBE5EC}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="27840" windowHeight="14868" activeTab="1" xr2:uid="{9F5E6FB9-32EF-42A5-B114-36A33DEBE5EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate Summary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="44">
   <si>
     <t>Plate Name</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Reagents</t>
+  </si>
+  <si>
+    <t>Q5 Master Mix</t>
   </si>
 </sst>
 </file>
@@ -561,13 +564,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +578,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -583,7 +586,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -591,7 +594,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -599,7 +602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -607,7 +610,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -615,7 +618,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -623,7 +626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -641,16 +644,16 @@
   <dimension ref="A1:J385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G95" sqref="G95"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="14.36328125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -682,7 +685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>_xlfn.CONCAT(B2,C2)</f>
         <v>A1</v>
@@ -703,7 +706,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="0">_xlfn.CONCAT(B3,C3)</f>
         <v>A2</v>
@@ -724,7 +727,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>A3</v>
@@ -745,7 +748,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>A4</v>
@@ -766,7 +769,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>A5</v>
@@ -787,7 +790,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>A6</v>
@@ -808,7 +811,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>A7</v>
@@ -829,7 +832,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>A8</v>
@@ -850,7 +853,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>A9</v>
@@ -871,7 +874,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>A10</v>
@@ -892,7 +895,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>A11</v>
@@ -913,7 +916,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>A12</v>
@@ -934,7 +937,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>A13</v>
@@ -955,7 +958,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>A14</v>
@@ -976,7 +979,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>A15</v>
@@ -997,7 +1000,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>A16</v>
@@ -1018,7 +1021,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>A17</v>
@@ -1039,7 +1042,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>A18</v>
@@ -1060,7 +1063,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>A19</v>
@@ -1081,7 +1084,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>A20</v>
@@ -1102,7 +1105,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>A21</v>
@@ -1123,7 +1126,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>A22</v>
@@ -1144,7 +1147,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>A23</v>
@@ -1165,7 +1168,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>A24</v>
@@ -1186,7 +1189,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>B1</v>
@@ -1207,7 +1210,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>B2</v>
@@ -1228,7 +1231,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>B3</v>
@@ -1249,7 +1252,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>B4</v>
@@ -1270,7 +1273,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>B5</v>
@@ -1291,7 +1294,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>B6</v>
@@ -1312,7 +1315,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>B7</v>
@@ -1333,7 +1336,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>B8</v>
@@ -1354,7 +1357,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>B9</v>
@@ -1375,7 +1378,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>B10</v>
@@ -1396,7 +1399,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>B11</v>
@@ -1417,7 +1420,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>B12</v>
@@ -1438,7 +1441,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>B13</v>
@@ -1459,7 +1462,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>B14</v>
@@ -1480,7 +1483,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>B15</v>
@@ -1501,7 +1504,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>B16</v>
@@ -1522,7 +1525,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>B17</v>
@@ -1543,7 +1546,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>B18</v>
@@ -1564,7 +1567,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>B19</v>
@@ -1585,7 +1588,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>B20</v>
@@ -1606,7 +1609,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>B21</v>
@@ -1627,7 +1630,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>B22</v>
@@ -1648,7 +1651,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>B23</v>
@@ -1669,7 +1672,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>B24</v>
@@ -1690,7 +1693,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>C1</v>
@@ -1711,7 +1714,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>C2</v>
@@ -1732,7 +1735,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>C3</v>
@@ -1753,7 +1756,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>C4</v>
@@ -1774,7 +1777,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>C5</v>
@@ -1795,7 +1798,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>C6</v>
@@ -1816,7 +1819,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>C7</v>
@@ -1837,7 +1840,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>C8</v>
@@ -1858,7 +1861,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>C9</v>
@@ -1879,7 +1882,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>C10</v>
@@ -1900,7 +1903,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>C11</v>
@@ -1921,7 +1924,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>C12</v>
@@ -1942,7 +1945,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>C13</v>
@@ -1963,7 +1966,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>C14</v>
@@ -1984,7 +1987,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>C15</v>
@@ -2005,7 +2008,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>C16</v>
@@ -2026,7 +2029,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>C17</v>
@@ -2047,7 +2050,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="str">
         <f t="shared" ref="A67:A130" si="1">_xlfn.CONCAT(B67,C67)</f>
         <v>C18</v>
@@ -2068,7 +2071,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="str">
         <f t="shared" si="1"/>
         <v>C19</v>
@@ -2089,7 +2092,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="str">
         <f t="shared" si="1"/>
         <v>C20</v>
@@ -2110,7 +2113,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="str">
         <f t="shared" si="1"/>
         <v>C21</v>
@@ -2131,7 +2134,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="str">
         <f t="shared" si="1"/>
         <v>C22</v>
@@ -2152,7 +2155,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="str">
         <f t="shared" si="1"/>
         <v>C23</v>
@@ -2173,7 +2176,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="str">
         <f t="shared" si="1"/>
         <v>C24</v>
@@ -2194,7 +2197,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="str">
         <f t="shared" si="1"/>
         <v>D1</v>
@@ -2215,7 +2218,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="str">
         <f t="shared" si="1"/>
         <v>D2</v>
@@ -2236,7 +2239,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="str">
         <f t="shared" si="1"/>
         <v>D3</v>
@@ -2257,7 +2260,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="str">
         <f t="shared" si="1"/>
         <v>D4</v>
@@ -2278,7 +2281,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="str">
         <f t="shared" si="1"/>
         <v>D5</v>
@@ -2299,7 +2302,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="str">
         <f t="shared" si="1"/>
         <v>D6</v>
@@ -2320,7 +2323,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="str">
         <f t="shared" si="1"/>
         <v>D7</v>
@@ -2341,7 +2344,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="str">
         <f t="shared" si="1"/>
         <v>D8</v>
@@ -2362,7 +2365,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="str">
         <f t="shared" si="1"/>
         <v>D9</v>
@@ -2383,7 +2386,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="str">
         <f t="shared" si="1"/>
         <v>D10</v>
@@ -2404,7 +2407,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="str">
         <f t="shared" si="1"/>
         <v>D11</v>
@@ -2425,7 +2428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="str">
         <f t="shared" si="1"/>
         <v>D12</v>
@@ -2446,7 +2449,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="str">
         <f t="shared" si="1"/>
         <v>D13</v>
@@ -2467,7 +2470,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="str">
         <f t="shared" si="1"/>
         <v>D14</v>
@@ -2488,7 +2491,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="str">
         <f t="shared" si="1"/>
         <v>D15</v>
@@ -2509,7 +2512,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="str">
         <f t="shared" si="1"/>
         <v>D16</v>
@@ -2530,7 +2533,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="str">
         <f t="shared" si="1"/>
         <v>D17</v>
@@ -2551,7 +2554,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="str">
         <f t="shared" si="1"/>
         <v>D18</v>
@@ -2572,7 +2575,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="str">
         <f t="shared" si="1"/>
         <v>D19</v>
@@ -2593,7 +2596,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="str">
         <f t="shared" si="1"/>
         <v>D20</v>
@@ -2614,7 +2617,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="str">
         <f t="shared" si="1"/>
         <v>D21</v>
@@ -2635,7 +2638,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="str">
         <f t="shared" si="1"/>
         <v>D22</v>
@@ -2656,7 +2659,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="str">
         <f t="shared" si="1"/>
         <v>D23</v>
@@ -2677,7 +2680,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="str">
         <f t="shared" si="1"/>
         <v>D24</v>
@@ -2698,7 +2701,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="str">
         <f t="shared" si="1"/>
         <v>E1</v>
@@ -2719,7 +2722,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2740,7 +2743,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="str">
         <f t="shared" si="1"/>
         <v>E3</v>
@@ -2761,7 +2764,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="str">
         <f t="shared" si="1"/>
         <v>E4</v>
@@ -2782,7 +2785,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="str">
         <f t="shared" si="1"/>
         <v>E5</v>
@@ -2803,7 +2806,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="str">
         <f t="shared" si="1"/>
         <v>E6</v>
@@ -2824,7 +2827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="str">
         <f t="shared" si="1"/>
         <v>E7</v>
@@ -2845,7 +2848,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="str">
         <f t="shared" si="1"/>
         <v>E8</v>
@@ -2866,7 +2869,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="str">
         <f t="shared" si="1"/>
         <v>E9</v>
@@ -2887,7 +2890,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="str">
         <f t="shared" si="1"/>
         <v>E10</v>
@@ -2908,7 +2911,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="str">
         <f t="shared" si="1"/>
         <v>E11</v>
@@ -2929,7 +2932,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="str">
         <f t="shared" si="1"/>
         <v>E12</v>
@@ -2950,7 +2953,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="str">
         <f t="shared" si="1"/>
         <v>E13</v>
@@ -2971,7 +2974,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="str">
         <f t="shared" si="1"/>
         <v>E14</v>
@@ -2992,7 +2995,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="str">
         <f t="shared" si="1"/>
         <v>E15</v>
@@ -3013,7 +3016,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="str">
         <f t="shared" si="1"/>
         <v>E16</v>
@@ -3034,7 +3037,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="str">
         <f t="shared" si="1"/>
         <v>E17</v>
@@ -3055,7 +3058,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="str">
         <f t="shared" si="1"/>
         <v>E18</v>
@@ -3076,7 +3079,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="str">
         <f t="shared" si="1"/>
         <v>E19</v>
@@ -3097,7 +3100,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="str">
         <f t="shared" si="1"/>
         <v>E20</v>
@@ -3118,7 +3121,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="str">
         <f t="shared" si="1"/>
         <v>E21</v>
@@ -3139,7 +3142,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="str">
         <f t="shared" si="1"/>
         <v>E22</v>
@@ -3160,7 +3163,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="str">
         <f t="shared" si="1"/>
         <v>E23</v>
@@ -3181,7 +3184,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="str">
         <f t="shared" si="1"/>
         <v>E24</v>
@@ -3202,7 +3205,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="str">
         <f t="shared" si="1"/>
         <v>F1</v>
@@ -3213,8 +3216,17 @@
       <c r="C122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D122" t="s">
+        <v>43</v>
+      </c>
+      <c r="E122">
+        <v>11</v>
+      </c>
+      <c r="I122" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="str">
         <f t="shared" si="1"/>
         <v>F2</v>
@@ -3225,8 +3237,17 @@
       <c r="C123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D123" t="s">
+        <v>43</v>
+      </c>
+      <c r="E123">
+        <v>11</v>
+      </c>
+      <c r="I123" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="str">
         <f t="shared" si="1"/>
         <v>F3</v>
@@ -3237,8 +3258,17 @@
       <c r="C124">
         <v>3</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D124" t="s">
+        <v>43</v>
+      </c>
+      <c r="E124">
+        <v>11</v>
+      </c>
+      <c r="I124" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="str">
         <f t="shared" si="1"/>
         <v>F4</v>
@@ -3249,8 +3279,17 @@
       <c r="C125">
         <v>4</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D125" t="s">
+        <v>43</v>
+      </c>
+      <c r="E125">
+        <v>11</v>
+      </c>
+      <c r="I125" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="str">
         <f t="shared" si="1"/>
         <v>F5</v>
@@ -3261,8 +3300,17 @@
       <c r="C126">
         <v>5</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D126" t="s">
+        <v>43</v>
+      </c>
+      <c r="E126">
+        <v>11</v>
+      </c>
+      <c r="I126" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="str">
         <f t="shared" si="1"/>
         <v>F6</v>
@@ -3273,8 +3321,17 @@
       <c r="C127">
         <v>6</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D127" t="s">
+        <v>43</v>
+      </c>
+      <c r="E127">
+        <v>11</v>
+      </c>
+      <c r="I127" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="str">
         <f t="shared" si="1"/>
         <v>F7</v>
@@ -3285,8 +3342,17 @@
       <c r="C128">
         <v>7</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D128" t="s">
+        <v>43</v>
+      </c>
+      <c r="E128">
+        <v>11</v>
+      </c>
+      <c r="I128" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="str">
         <f t="shared" si="1"/>
         <v>F8</v>
@@ -3297,8 +3363,17 @@
       <c r="C129">
         <v>8</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D129" t="s">
+        <v>43</v>
+      </c>
+      <c r="E129">
+        <v>11</v>
+      </c>
+      <c r="I129" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="str">
         <f t="shared" si="1"/>
         <v>F9</v>
@@ -3309,8 +3384,17 @@
       <c r="C130">
         <v>9</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D130" t="s">
+        <v>43</v>
+      </c>
+      <c r="E130">
+        <v>11</v>
+      </c>
+      <c r="I130" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="str">
         <f t="shared" ref="A131:A194" si="2">_xlfn.CONCAT(B131,C131)</f>
         <v>F10</v>
@@ -3321,8 +3405,17 @@
       <c r="C131">
         <v>10</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D131" t="s">
+        <v>43</v>
+      </c>
+      <c r="E131">
+        <v>11</v>
+      </c>
+      <c r="I131" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="str">
         <f t="shared" si="2"/>
         <v>F11</v>
@@ -3333,8 +3426,17 @@
       <c r="C132">
         <v>11</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D132" t="s">
+        <v>43</v>
+      </c>
+      <c r="E132">
+        <v>11</v>
+      </c>
+      <c r="I132" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="str">
         <f t="shared" si="2"/>
         <v>F12</v>
@@ -3345,8 +3447,17 @@
       <c r="C133">
         <v>12</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D133" t="s">
+        <v>43</v>
+      </c>
+      <c r="E133">
+        <v>11</v>
+      </c>
+      <c r="I133" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="str">
         <f t="shared" si="2"/>
         <v>F13</v>
@@ -3357,8 +3468,17 @@
       <c r="C134">
         <v>13</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D134" t="s">
+        <v>43</v>
+      </c>
+      <c r="E134">
+        <v>11</v>
+      </c>
+      <c r="I134" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="str">
         <f t="shared" si="2"/>
         <v>F14</v>
@@ -3369,8 +3489,17 @@
       <c r="C135">
         <v>14</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D135" t="s">
+        <v>43</v>
+      </c>
+      <c r="E135">
+        <v>11</v>
+      </c>
+      <c r="I135" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="str">
         <f t="shared" si="2"/>
         <v>F15</v>
@@ -3381,8 +3510,17 @@
       <c r="C136">
         <v>15</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D136" t="s">
+        <v>43</v>
+      </c>
+      <c r="E136">
+        <v>11</v>
+      </c>
+      <c r="I136" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="str">
         <f t="shared" si="2"/>
         <v>F16</v>
@@ -3393,8 +3531,17 @@
       <c r="C137">
         <v>16</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D137" t="s">
+        <v>43</v>
+      </c>
+      <c r="E137">
+        <v>11</v>
+      </c>
+      <c r="I137" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="str">
         <f t="shared" si="2"/>
         <v>F17</v>
@@ -3405,8 +3552,17 @@
       <c r="C138">
         <v>17</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D138" t="s">
+        <v>43</v>
+      </c>
+      <c r="E138">
+        <v>11</v>
+      </c>
+      <c r="I138" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="str">
         <f t="shared" si="2"/>
         <v>F18</v>
@@ -3417,8 +3573,17 @@
       <c r="C139">
         <v>18</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D139" t="s">
+        <v>43</v>
+      </c>
+      <c r="E139">
+        <v>11</v>
+      </c>
+      <c r="I139" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="str">
         <f t="shared" si="2"/>
         <v>F19</v>
@@ -3429,8 +3594,17 @@
       <c r="C140">
         <v>19</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D140" t="s">
+        <v>43</v>
+      </c>
+      <c r="E140">
+        <v>11</v>
+      </c>
+      <c r="I140" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="str">
         <f t="shared" si="2"/>
         <v>F20</v>
@@ -3441,8 +3615,17 @@
       <c r="C141">
         <v>20</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D141" t="s">
+        <v>43</v>
+      </c>
+      <c r="E141">
+        <v>11</v>
+      </c>
+      <c r="I141" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="str">
         <f t="shared" si="2"/>
         <v>F21</v>
@@ -3453,8 +3636,17 @@
       <c r="C142">
         <v>21</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D142" t="s">
+        <v>43</v>
+      </c>
+      <c r="E142">
+        <v>11</v>
+      </c>
+      <c r="I142" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="str">
         <f t="shared" si="2"/>
         <v>F22</v>
@@ -3465,8 +3657,17 @@
       <c r="C143">
         <v>22</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D143" t="s">
+        <v>43</v>
+      </c>
+      <c r="E143">
+        <v>11</v>
+      </c>
+      <c r="I143" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="str">
         <f t="shared" si="2"/>
         <v>F23</v>
@@ -3477,8 +3678,17 @@
       <c r="C144">
         <v>23</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D144" t="s">
+        <v>43</v>
+      </c>
+      <c r="E144">
+        <v>11</v>
+      </c>
+      <c r="I144" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="str">
         <f t="shared" si="2"/>
         <v>F24</v>
@@ -3489,8 +3699,17 @@
       <c r="C145">
         <v>24</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D145" t="s">
+        <v>43</v>
+      </c>
+      <c r="E145">
+        <v>11</v>
+      </c>
+      <c r="I145" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="str">
         <f t="shared" si="2"/>
         <v>G1</v>
@@ -3502,7 +3721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="str">
         <f t="shared" si="2"/>
         <v>G2</v>
@@ -3514,7 +3733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="str">
         <f t="shared" si="2"/>
         <v>G3</v>
@@ -3526,7 +3745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="str">
         <f t="shared" si="2"/>
         <v>G4</v>
@@ -3538,7 +3757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="str">
         <f t="shared" si="2"/>
         <v>G5</v>
@@ -3550,7 +3769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="str">
         <f t="shared" si="2"/>
         <v>G6</v>
@@ -3562,7 +3781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="str">
         <f t="shared" si="2"/>
         <v>G7</v>
@@ -3574,7 +3793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="str">
         <f t="shared" si="2"/>
         <v>G8</v>
@@ -3586,7 +3805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="str">
         <f t="shared" si="2"/>
         <v>G9</v>
@@ -3598,7 +3817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="str">
         <f t="shared" si="2"/>
         <v>G10</v>
@@ -3610,7 +3829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="str">
         <f t="shared" si="2"/>
         <v>G11</v>
@@ -3622,7 +3841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="str">
         <f t="shared" si="2"/>
         <v>G12</v>
@@ -3634,7 +3853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="str">
         <f t="shared" si="2"/>
         <v>G13</v>
@@ -3646,7 +3865,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="str">
         <f t="shared" si="2"/>
         <v>G14</v>
@@ -3658,7 +3877,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="str">
         <f t="shared" si="2"/>
         <v>G15</v>
@@ -3670,7 +3889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="str">
         <f t="shared" si="2"/>
         <v>G16</v>
@@ -3682,7 +3901,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="str">
         <f t="shared" si="2"/>
         <v>G17</v>
@@ -3694,7 +3913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="str">
         <f t="shared" si="2"/>
         <v>G18</v>
@@ -3706,7 +3925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="str">
         <f t="shared" si="2"/>
         <v>G19</v>
@@ -3718,7 +3937,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="str">
         <f t="shared" si="2"/>
         <v>G20</v>
@@ -3730,7 +3949,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="str">
         <f t="shared" si="2"/>
         <v>G21</v>
@@ -3742,7 +3961,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="str">
         <f t="shared" si="2"/>
         <v>G22</v>
@@ -3754,7 +3973,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="str">
         <f t="shared" si="2"/>
         <v>G23</v>
@@ -3766,7 +3985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="str">
         <f t="shared" si="2"/>
         <v>G24</v>
@@ -3778,7 +3997,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="str">
         <f t="shared" si="2"/>
         <v>H1</v>
@@ -3790,7 +4009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="str">
         <f t="shared" si="2"/>
         <v>H2</v>
@@ -3802,7 +4021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="str">
         <f t="shared" si="2"/>
         <v>H3</v>
@@ -3814,7 +4033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="str">
         <f t="shared" si="2"/>
         <v>H4</v>
@@ -3826,7 +4045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="str">
         <f t="shared" si="2"/>
         <v>H5</v>
@@ -3838,7 +4057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="str">
         <f t="shared" si="2"/>
         <v>H6</v>
@@ -3850,7 +4069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="str">
         <f t="shared" si="2"/>
         <v>H7</v>
@@ -3862,7 +4081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="str">
         <f t="shared" si="2"/>
         <v>H8</v>
@@ -3874,7 +4093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="str">
         <f t="shared" si="2"/>
         <v>H9</v>
@@ -3886,7 +4105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="str">
         <f t="shared" si="2"/>
         <v>H10</v>
@@ -3898,7 +4117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="str">
         <f t="shared" si="2"/>
         <v>H11</v>
@@ -3910,7 +4129,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="str">
         <f t="shared" si="2"/>
         <v>H12</v>
@@ -3922,7 +4141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="str">
         <f t="shared" si="2"/>
         <v>H13</v>
@@ -3934,7 +4153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="str">
         <f t="shared" si="2"/>
         <v>H14</v>
@@ -3946,7 +4165,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="str">
         <f t="shared" si="2"/>
         <v>H15</v>
@@ -3958,7 +4177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="str">
         <f t="shared" si="2"/>
         <v>H16</v>
@@ -3970,7 +4189,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="str">
         <f t="shared" si="2"/>
         <v>H17</v>
@@ -3982,7 +4201,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="str">
         <f t="shared" si="2"/>
         <v>H18</v>
@@ -3994,7 +4213,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="str">
         <f t="shared" si="2"/>
         <v>H19</v>
@@ -4006,7 +4225,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="str">
         <f t="shared" si="2"/>
         <v>H20</v>
@@ -4018,7 +4237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="str">
         <f t="shared" si="2"/>
         <v>H21</v>
@@ -4030,7 +4249,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="str">
         <f t="shared" si="2"/>
         <v>H22</v>
@@ -4042,7 +4261,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="str">
         <f t="shared" si="2"/>
         <v>H23</v>
@@ -4054,7 +4273,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="str">
         <f t="shared" si="2"/>
         <v>H24</v>
@@ -4066,7 +4285,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="str">
         <f t="shared" si="2"/>
         <v>I1</v>
@@ -4078,7 +4297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="str">
         <f t="shared" ref="A195:A258" si="3">_xlfn.CONCAT(B195,C195)</f>
         <v>I2</v>
@@ -4090,7 +4309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="str">
         <f t="shared" si="3"/>
         <v>I3</v>
@@ -4102,7 +4321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="str">
         <f t="shared" si="3"/>
         <v>I4</v>
@@ -4114,7 +4333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="str">
         <f t="shared" si="3"/>
         <v>I5</v>
@@ -4126,7 +4345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="str">
         <f t="shared" si="3"/>
         <v>I6</v>
@@ -4138,7 +4357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="str">
         <f t="shared" si="3"/>
         <v>I7</v>
@@ -4150,7 +4369,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="str">
         <f t="shared" si="3"/>
         <v>I8</v>
@@ -4162,7 +4381,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="str">
         <f t="shared" si="3"/>
         <v>I9</v>
@@ -4174,7 +4393,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="str">
         <f t="shared" si="3"/>
         <v>I10</v>
@@ -4186,7 +4405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="str">
         <f t="shared" si="3"/>
         <v>I11</v>
@@ -4198,7 +4417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="str">
         <f t="shared" si="3"/>
         <v>I12</v>
@@ -4210,7 +4429,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="str">
         <f t="shared" si="3"/>
         <v>I13</v>
@@ -4222,7 +4441,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="str">
         <f t="shared" si="3"/>
         <v>I14</v>
@@ -4234,7 +4453,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="str">
         <f t="shared" si="3"/>
         <v>I15</v>
@@ -4246,7 +4465,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="str">
         <f t="shared" si="3"/>
         <v>I16</v>
@@ -4258,7 +4477,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="str">
         <f t="shared" si="3"/>
         <v>I17</v>
@@ -4270,7 +4489,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="str">
         <f t="shared" si="3"/>
         <v>I18</v>
@@ -4282,7 +4501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="str">
         <f t="shared" si="3"/>
         <v>I19</v>
@@ -4294,7 +4513,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="str">
         <f t="shared" si="3"/>
         <v>I20</v>
@@ -4306,7 +4525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="str">
         <f t="shared" si="3"/>
         <v>I21</v>
@@ -4318,7 +4537,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="str">
         <f t="shared" si="3"/>
         <v>I22</v>
@@ -4330,7 +4549,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="str">
         <f t="shared" si="3"/>
         <v>I23</v>
@@ -4342,7 +4561,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="str">
         <f t="shared" si="3"/>
         <v>I24</v>
@@ -4354,7 +4573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="str">
         <f t="shared" si="3"/>
         <v>J1</v>
@@ -4366,7 +4585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="str">
         <f t="shared" si="3"/>
         <v>J2</v>
@@ -4378,7 +4597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="str">
         <f t="shared" si="3"/>
         <v>J3</v>
@@ -4390,7 +4609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="str">
         <f t="shared" si="3"/>
         <v>J4</v>
@@ -4402,7 +4621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="str">
         <f t="shared" si="3"/>
         <v>J5</v>
@@ -4414,7 +4633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="str">
         <f t="shared" si="3"/>
         <v>J6</v>
@@ -4426,7 +4645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="str">
         <f t="shared" si="3"/>
         <v>J7</v>
@@ -4438,7 +4657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="str">
         <f t="shared" si="3"/>
         <v>J8</v>
@@ -4450,7 +4669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="str">
         <f t="shared" si="3"/>
         <v>J9</v>
@@ -4462,7 +4681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="str">
         <f t="shared" si="3"/>
         <v>J10</v>
@@ -4474,7 +4693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="str">
         <f t="shared" si="3"/>
         <v>J11</v>
@@ -4486,7 +4705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="str">
         <f t="shared" si="3"/>
         <v>J12</v>
@@ -4498,7 +4717,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="str">
         <f t="shared" si="3"/>
         <v>J13</v>
@@ -4510,7 +4729,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="str">
         <f t="shared" si="3"/>
         <v>J14</v>
@@ -4522,7 +4741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="str">
         <f t="shared" si="3"/>
         <v>J15</v>
@@ -4534,7 +4753,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="str">
         <f t="shared" si="3"/>
         <v>J16</v>
@@ -4546,7 +4765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="str">
         <f t="shared" si="3"/>
         <v>J17</v>
@@ -4558,7 +4777,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="str">
         <f t="shared" si="3"/>
         <v>J18</v>
@@ -4570,7 +4789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="str">
         <f t="shared" si="3"/>
         <v>J19</v>
@@ -4582,7 +4801,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="str">
         <f t="shared" si="3"/>
         <v>J20</v>
@@ -4594,7 +4813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="str">
         <f t="shared" si="3"/>
         <v>J21</v>
@@ -4606,7 +4825,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="str">
         <f t="shared" si="3"/>
         <v>J22</v>
@@ -4618,7 +4837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="str">
         <f t="shared" si="3"/>
         <v>J23</v>
@@ -4630,7 +4849,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="str">
         <f t="shared" si="3"/>
         <v>J24</v>
@@ -4642,7 +4861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="str">
         <f t="shared" si="3"/>
         <v>K1</v>
@@ -4654,7 +4873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="str">
         <f t="shared" si="3"/>
         <v>K2</v>
@@ -4666,7 +4885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="str">
         <f t="shared" si="3"/>
         <v>K3</v>
@@ -4678,7 +4897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="str">
         <f t="shared" si="3"/>
         <v>K4</v>
@@ -4690,7 +4909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="str">
         <f t="shared" si="3"/>
         <v>K5</v>
@@ -4702,7 +4921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" t="str">
         <f t="shared" si="3"/>
         <v>K6</v>
@@ -4714,7 +4933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="str">
         <f t="shared" si="3"/>
         <v>K7</v>
@@ -4726,7 +4945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="str">
         <f t="shared" si="3"/>
         <v>K8</v>
@@ -4738,7 +4957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="str">
         <f t="shared" si="3"/>
         <v>K9</v>
@@ -4750,7 +4969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="str">
         <f t="shared" si="3"/>
         <v>K10</v>
@@ -4762,7 +4981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="str">
         <f t="shared" si="3"/>
         <v>K11</v>
@@ -4774,7 +4993,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="str">
         <f t="shared" si="3"/>
         <v>K12</v>
@@ -4786,7 +5005,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="str">
         <f t="shared" si="3"/>
         <v>K13</v>
@@ -4798,7 +5017,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" t="str">
         <f t="shared" si="3"/>
         <v>K14</v>
@@ -4810,7 +5029,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" t="str">
         <f t="shared" si="3"/>
         <v>K15</v>
@@ -4822,7 +5041,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" t="str">
         <f t="shared" si="3"/>
         <v>K16</v>
@@ -4834,7 +5053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" t="str">
         <f t="shared" si="3"/>
         <v>K17</v>
@@ -4846,7 +5065,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" t="str">
         <f t="shared" ref="A259:A322" si="4">_xlfn.CONCAT(B259,C259)</f>
         <v>K18</v>
@@ -4858,7 +5077,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="str">
         <f t="shared" si="4"/>
         <v>K19</v>
@@ -4870,7 +5089,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" t="str">
         <f t="shared" si="4"/>
         <v>K20</v>
@@ -4882,7 +5101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" t="str">
         <f t="shared" si="4"/>
         <v>K21</v>
@@ -4894,7 +5113,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" t="str">
         <f t="shared" si="4"/>
         <v>K22</v>
@@ -4906,7 +5125,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" t="str">
         <f t="shared" si="4"/>
         <v>K23</v>
@@ -4918,7 +5137,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" t="str">
         <f t="shared" si="4"/>
         <v>K24</v>
@@ -4930,7 +5149,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" t="str">
         <f t="shared" si="4"/>
         <v>L1</v>
@@ -4942,7 +5161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" t="str">
         <f t="shared" si="4"/>
         <v>L2</v>
@@ -4954,7 +5173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" t="str">
         <f t="shared" si="4"/>
         <v>L3</v>
@@ -4966,7 +5185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" t="str">
         <f t="shared" si="4"/>
         <v>L4</v>
@@ -4978,7 +5197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" t="str">
         <f t="shared" si="4"/>
         <v>L5</v>
@@ -4990,7 +5209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" t="str">
         <f t="shared" si="4"/>
         <v>L6</v>
@@ -5002,7 +5221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" t="str">
         <f t="shared" si="4"/>
         <v>L7</v>
@@ -5014,7 +5233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" t="str">
         <f t="shared" si="4"/>
         <v>L8</v>
@@ -5026,7 +5245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" t="str">
         <f t="shared" si="4"/>
         <v>L9</v>
@@ -5038,7 +5257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" t="str">
         <f t="shared" si="4"/>
         <v>L10</v>
@@ -5050,7 +5269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" t="str">
         <f t="shared" si="4"/>
         <v>L11</v>
@@ -5062,7 +5281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="str">
         <f t="shared" si="4"/>
         <v>L12</v>
@@ -5074,7 +5293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" t="str">
         <f t="shared" si="4"/>
         <v>L13</v>
@@ -5086,7 +5305,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" t="str">
         <f t="shared" si="4"/>
         <v>L14</v>
@@ -5098,7 +5317,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" t="str">
         <f t="shared" si="4"/>
         <v>L15</v>
@@ -5110,7 +5329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="str">
         <f t="shared" si="4"/>
         <v>L16</v>
@@ -5122,7 +5341,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" t="str">
         <f t="shared" si="4"/>
         <v>L17</v>
@@ -5134,7 +5353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" t="str">
         <f t="shared" si="4"/>
         <v>L18</v>
@@ -5146,7 +5365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" t="str">
         <f t="shared" si="4"/>
         <v>L19</v>
@@ -5158,7 +5377,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" t="str">
         <f t="shared" si="4"/>
         <v>L20</v>
@@ -5170,7 +5389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" t="str">
         <f t="shared" si="4"/>
         <v>L21</v>
@@ -5182,7 +5401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" t="str">
         <f t="shared" si="4"/>
         <v>L22</v>
@@ -5194,7 +5413,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" t="str">
         <f t="shared" si="4"/>
         <v>L23</v>
@@ -5206,7 +5425,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" t="str">
         <f t="shared" si="4"/>
         <v>L24</v>
@@ -5218,7 +5437,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" t="str">
         <f t="shared" si="4"/>
         <v>M1</v>
@@ -5230,7 +5449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" t="str">
         <f t="shared" si="4"/>
         <v>M2</v>
@@ -5242,7 +5461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" t="str">
         <f t="shared" si="4"/>
         <v>M3</v>
@@ -5254,7 +5473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" t="str">
         <f t="shared" si="4"/>
         <v>M4</v>
@@ -5266,7 +5485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" t="str">
         <f t="shared" si="4"/>
         <v>M5</v>
@@ -5278,7 +5497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295" t="str">
         <f t="shared" si="4"/>
         <v>M6</v>
@@ -5290,7 +5509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" t="str">
         <f t="shared" si="4"/>
         <v>M7</v>
@@ -5302,7 +5521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" t="str">
         <f t="shared" si="4"/>
         <v>M8</v>
@@ -5314,7 +5533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" t="str">
         <f t="shared" si="4"/>
         <v>M9</v>
@@ -5326,7 +5545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" t="str">
         <f t="shared" si="4"/>
         <v>M10</v>
@@ -5338,7 +5557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" t="str">
         <f t="shared" si="4"/>
         <v>M11</v>
@@ -5350,7 +5569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" t="str">
         <f t="shared" si="4"/>
         <v>M12</v>
@@ -5362,7 +5581,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" t="str">
         <f t="shared" si="4"/>
         <v>M13</v>
@@ -5374,7 +5593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303" t="str">
         <f t="shared" si="4"/>
         <v>M14</v>
@@ -5386,7 +5605,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304" t="str">
         <f t="shared" si="4"/>
         <v>M15</v>
@@ -5398,7 +5617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305" t="str">
         <f t="shared" si="4"/>
         <v>M16</v>
@@ -5410,7 +5629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" t="str">
         <f t="shared" si="4"/>
         <v>M17</v>
@@ -5422,7 +5641,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" t="str">
         <f t="shared" si="4"/>
         <v>M18</v>
@@ -5434,7 +5653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" t="str">
         <f t="shared" si="4"/>
         <v>M19</v>
@@ -5446,7 +5665,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" t="str">
         <f t="shared" si="4"/>
         <v>M20</v>
@@ -5458,7 +5677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310" t="str">
         <f t="shared" si="4"/>
         <v>M21</v>
@@ -5470,7 +5689,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A311" t="str">
         <f t="shared" si="4"/>
         <v>M22</v>
@@ -5482,7 +5701,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A312" t="str">
         <f t="shared" si="4"/>
         <v>M23</v>
@@ -5494,7 +5713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" t="str">
         <f t="shared" si="4"/>
         <v>M24</v>
@@ -5506,7 +5725,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314" t="str">
         <f t="shared" si="4"/>
         <v>N1</v>
@@ -5518,7 +5737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315" t="str">
         <f t="shared" si="4"/>
         <v>N2</v>
@@ -5530,7 +5749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316" t="str">
         <f t="shared" si="4"/>
         <v>N3</v>
@@ -5542,7 +5761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" t="str">
         <f t="shared" si="4"/>
         <v>N4</v>
@@ -5554,7 +5773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" t="str">
         <f t="shared" si="4"/>
         <v>N5</v>
@@ -5566,7 +5785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" t="str">
         <f t="shared" si="4"/>
         <v>N6</v>
@@ -5578,7 +5797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" t="str">
         <f t="shared" si="4"/>
         <v>N7</v>
@@ -5590,7 +5809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321" t="str">
         <f t="shared" si="4"/>
         <v>N8</v>
@@ -5602,7 +5821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322" t="str">
         <f t="shared" si="4"/>
         <v>N9</v>
@@ -5614,7 +5833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323" t="str">
         <f t="shared" ref="A323:A385" si="5">_xlfn.CONCAT(B323,C323)</f>
         <v>N10</v>
@@ -5626,7 +5845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A324" t="str">
         <f t="shared" si="5"/>
         <v>N11</v>
@@ -5638,7 +5857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325" t="str">
         <f t="shared" si="5"/>
         <v>N12</v>
@@ -5650,7 +5869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326" t="str">
         <f t="shared" si="5"/>
         <v>N13</v>
@@ -5662,7 +5881,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A327" t="str">
         <f t="shared" si="5"/>
         <v>N14</v>
@@ -5674,7 +5893,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328" t="str">
         <f t="shared" si="5"/>
         <v>N15</v>
@@ -5686,7 +5905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329" t="str">
         <f t="shared" si="5"/>
         <v>N16</v>
@@ -5698,7 +5917,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330" t="str">
         <f t="shared" si="5"/>
         <v>N17</v>
@@ -5710,7 +5929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331" t="str">
         <f t="shared" si="5"/>
         <v>N18</v>
@@ -5722,7 +5941,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" t="str">
         <f t="shared" si="5"/>
         <v>N19</v>
@@ -5734,7 +5953,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333" t="str">
         <f t="shared" si="5"/>
         <v>N20</v>
@@ -5746,7 +5965,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334" t="str">
         <f t="shared" si="5"/>
         <v>N21</v>
@@ -5758,7 +5977,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335" t="str">
         <f t="shared" si="5"/>
         <v>N22</v>
@@ -5770,7 +5989,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336" t="str">
         <f t="shared" si="5"/>
         <v>N23</v>
@@ -5782,7 +6001,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" t="str">
         <f t="shared" si="5"/>
         <v>N24</v>
@@ -5794,7 +6013,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" t="str">
         <f t="shared" si="5"/>
         <v>O1</v>
@@ -5806,7 +6025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339" t="str">
         <f t="shared" si="5"/>
         <v>O2</v>
@@ -5818,7 +6037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" t="str">
         <f t="shared" si="5"/>
         <v>O3</v>
@@ -5830,7 +6049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341" t="str">
         <f t="shared" si="5"/>
         <v>O4</v>
@@ -5842,7 +6061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342" t="str">
         <f t="shared" si="5"/>
         <v>O5</v>
@@ -5854,7 +6073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" t="str">
         <f t="shared" si="5"/>
         <v>O6</v>
@@ -5866,7 +6085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344" t="str">
         <f t="shared" si="5"/>
         <v>O7</v>
@@ -5878,7 +6097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345" t="str">
         <f t="shared" si="5"/>
         <v>O8</v>
@@ -5890,7 +6109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A346" t="str">
         <f t="shared" si="5"/>
         <v>O9</v>
@@ -5902,7 +6121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A347" t="str">
         <f t="shared" si="5"/>
         <v>O10</v>
@@ -5914,7 +6133,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348" t="str">
         <f t="shared" si="5"/>
         <v>O11</v>
@@ -5926,7 +6145,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349" t="str">
         <f t="shared" si="5"/>
         <v>O12</v>
@@ -5938,7 +6157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350" t="str">
         <f t="shared" si="5"/>
         <v>O13</v>
@@ -5950,7 +6169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351" t="str">
         <f t="shared" si="5"/>
         <v>O14</v>
@@ -5962,7 +6181,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352" t="str">
         <f t="shared" si="5"/>
         <v>O15</v>
@@ -5974,7 +6193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A353" t="str">
         <f t="shared" si="5"/>
         <v>O16</v>
@@ -5986,7 +6205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A354" t="str">
         <f t="shared" si="5"/>
         <v>O17</v>
@@ -5998,7 +6217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A355" t="str">
         <f t="shared" si="5"/>
         <v>O18</v>
@@ -6010,7 +6229,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A356" t="str">
         <f t="shared" si="5"/>
         <v>O19</v>
@@ -6022,7 +6241,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A357" t="str">
         <f t="shared" si="5"/>
         <v>O20</v>
@@ -6034,7 +6253,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A358" t="str">
         <f t="shared" si="5"/>
         <v>O21</v>
@@ -6046,7 +6265,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A359" t="str">
         <f t="shared" si="5"/>
         <v>O22</v>
@@ -6058,7 +6277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A360" t="str">
         <f t="shared" si="5"/>
         <v>O23</v>
@@ -6070,7 +6289,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A361" t="str">
         <f t="shared" si="5"/>
         <v>O24</v>
@@ -6082,7 +6301,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A362" t="str">
         <f t="shared" si="5"/>
         <v>P1</v>
@@ -6094,7 +6313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A363" t="str">
         <f t="shared" si="5"/>
         <v>P2</v>
@@ -6106,7 +6325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A364" t="str">
         <f t="shared" si="5"/>
         <v>P3</v>
@@ -6118,7 +6337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A365" t="str">
         <f t="shared" si="5"/>
         <v>P4</v>
@@ -6130,7 +6349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A366" t="str">
         <f t="shared" si="5"/>
         <v>P5</v>
@@ -6142,7 +6361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A367" t="str">
         <f t="shared" si="5"/>
         <v>P6</v>
@@ -6154,7 +6373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A368" t="str">
         <f t="shared" si="5"/>
         <v>P7</v>
@@ -6166,7 +6385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A369" t="str">
         <f t="shared" si="5"/>
         <v>P8</v>
@@ -6178,7 +6397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A370" t="str">
         <f t="shared" si="5"/>
         <v>P9</v>
@@ -6190,7 +6409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A371" t="str">
         <f t="shared" si="5"/>
         <v>P10</v>
@@ -6202,7 +6421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A372" t="str">
         <f t="shared" si="5"/>
         <v>P11</v>
@@ -6214,7 +6433,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A373" t="str">
         <f t="shared" si="5"/>
         <v>P12</v>
@@ -6226,7 +6445,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A374" t="str">
         <f t="shared" si="5"/>
         <v>P13</v>
@@ -6238,7 +6457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A375" t="str">
         <f t="shared" si="5"/>
         <v>P14</v>
@@ -6250,7 +6469,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A376" t="str">
         <f t="shared" si="5"/>
         <v>P15</v>
@@ -6262,7 +6481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A377" t="str">
         <f t="shared" si="5"/>
         <v>P16</v>
@@ -6274,7 +6493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A378" t="str">
         <f t="shared" si="5"/>
         <v>P17</v>
@@ -6286,7 +6505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A379" t="str">
         <f t="shared" si="5"/>
         <v>P18</v>
@@ -6298,7 +6517,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A380" t="str">
         <f t="shared" si="5"/>
         <v>P19</v>
@@ -6310,7 +6529,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A381" t="str">
         <f t="shared" si="5"/>
         <v>P20</v>
@@ -6322,7 +6541,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A382" t="str">
         <f t="shared" si="5"/>
         <v>P21</v>
@@ -6334,7 +6553,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A383" t="str">
         <f t="shared" si="5"/>
         <v>P22</v>
@@ -6346,7 +6565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A384" t="str">
         <f t="shared" si="5"/>
         <v>P23</v>
@@ -6358,7 +6577,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385" t="str">
         <f t="shared" si="5"/>
         <v>P24</v>

</xml_diff>